<commit_message>
slight code tweaks and derived objects for 2024 results
</commit_message>
<xml_diff>
--- a/outgoing/PITcleanr/UC_Steelhead_2024_OKL.xlsx
+++ b/outgoing/PITcleanr/UC_Steelhead_2024_OKL.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P1153"/>
+  <dimension ref="A1:P1137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -67720,7 +67720,7 @@
     <row r="1115">
       <c r="A1115" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1115" t="inlineStr">
@@ -67733,23 +67733,26 @@
       </c>
       <c r="D1115" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Recapture</t>
         </is>
       </c>
       <c r="E1115">
         <v>1</v>
       </c>
       <c r="F1115" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="G1115" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="H1115">
         <v>0</v>
       </c>
+      <c r="I1115">
+        <v>4.3</v>
+      </c>
       <c r="J1115" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1115">
         <v>1</v>
@@ -67766,17 +67769,20 @@
       </c>
       <c r="N1115" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1115" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1115" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1116">
       <c r="A1116" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1116" t="inlineStr">
@@ -67796,19 +67802,19 @@
         <v>2</v>
       </c>
       <c r="F1116" s="2">
-        <v>45100.84309027778</v>
+        <v>45181.34018518518</v>
       </c>
       <c r="G1116" s="2">
-        <v>45100.84549768519</v>
+        <v>45181.34247685185</v>
       </c>
       <c r="H1116">
-        <v>3.466666666666667</v>
+        <v>3.3</v>
       </c>
       <c r="I1116">
-        <v>292.4333333333333</v>
+        <v>46.46666666666667</v>
       </c>
       <c r="J1116" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1116">
         <v>1</v>
@@ -67825,17 +67831,20 @@
       </c>
       <c r="N1116" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1116" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1116" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1117">
       <c r="A1117" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1117" t="inlineStr">
@@ -67852,22 +67861,22 @@
         </is>
       </c>
       <c r="E1117">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F1117" s="2">
-        <v>45105.67033564814</v>
+        <v>45186.11847222222</v>
       </c>
       <c r="G1117" s="2">
-        <v>45105.67413194444</v>
+        <v>45186.16163194444</v>
       </c>
       <c r="H1117">
-        <v>5.466666666666667</v>
+        <v>62.15</v>
       </c>
       <c r="I1117">
-        <v>6947.766666666666</v>
+        <v>6877.433333333333</v>
       </c>
       <c r="J1117" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1117">
         <v>2</v>
@@ -67884,17 +67893,20 @@
       </c>
       <c r="N1117" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1117" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1117" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1118">
       <c r="A1118" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1118" t="inlineStr">
@@ -67911,22 +67923,22 @@
         </is>
       </c>
       <c r="E1118">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F1118" s="2">
-        <v>45107.18331018518</v>
+        <v>45187.44148148148</v>
       </c>
       <c r="G1118" s="2">
-        <v>45107.18732638888</v>
+        <v>45187.45084490741</v>
       </c>
       <c r="H1118">
-        <v>5.783333333333333</v>
+        <v>13.48333333333333</v>
       </c>
       <c r="I1118">
-        <v>2173.216666666667</v>
+        <v>1842.983333333333</v>
       </c>
       <c r="J1118" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1118">
         <v>3</v>
@@ -67943,17 +67955,20 @@
       </c>
       <c r="N1118" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1118" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1118" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1119">
       <c r="A1119" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1119" t="inlineStr">
@@ -67973,19 +67988,19 @@
         <v>3</v>
       </c>
       <c r="F1119" s="2">
-        <v>45109.58233796296</v>
+        <v>45189.72104166666</v>
       </c>
       <c r="G1119" s="2">
-        <v>45109.64785879629</v>
+        <v>45189.77603009259</v>
       </c>
       <c r="H1119">
-        <v>94.34999999999999</v>
+        <v>79.18333333333334</v>
       </c>
       <c r="I1119">
-        <v>3448.816666666667</v>
+        <v>3269.083333333333</v>
       </c>
       <c r="J1119" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1119">
         <v>4</v>
@@ -68002,17 +68017,20 @@
       </c>
       <c r="N1119" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1119" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1119" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1120">
       <c r="A1120" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1120" t="inlineStr">
@@ -68032,19 +68050,19 @@
         <v>1</v>
       </c>
       <c r="F1120" s="2">
-        <v>45197.82210648149</v>
+        <v>45203.8422337963</v>
       </c>
       <c r="G1120" s="2">
-        <v>45197.82210648149</v>
+        <v>45203.8422337963</v>
       </c>
       <c r="H1120">
         <v>0</v>
       </c>
       <c r="I1120">
-        <v>126970.9166666667</v>
+        <v>20255.33333333333</v>
       </c>
       <c r="J1120" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1120">
         <v>5</v>
@@ -68061,17 +68079,20 @@
       </c>
       <c r="N1120" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1120" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P1120" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1121">
       <c r="A1121" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1121" t="inlineStr">
@@ -68088,22 +68109,22 @@
         </is>
       </c>
       <c r="E1121">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1121" s="2">
-        <v>45197.82258101852</v>
+        <v>45203.84256944444</v>
       </c>
       <c r="G1121" s="2">
-        <v>45351.23668981482</v>
+        <v>45203.84256944444</v>
       </c>
       <c r="H1121">
-        <v>220916.3166666667</v>
+        <v>0</v>
       </c>
       <c r="I1121">
-        <v>0.6833333333333333</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="J1121" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1121">
         <v>6</v>
@@ -68120,22 +68141,25 @@
       </c>
       <c r="N1121" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1121" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P1121" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1122">
       <c r="A1122" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1122" t="inlineStr">
         <is>
-          <t>OKL_D</t>
+          <t>BPC_D</t>
         </is>
       </c>
       <c r="C1122">
@@ -68150,51 +68174,54 @@
         <v>1</v>
       </c>
       <c r="F1122" s="2">
-        <v>45351.23675925926</v>
+        <v>45419.55473379629</v>
       </c>
       <c r="G1122" s="2">
-        <v>45351.23675925926</v>
+        <v>45419.55473379629</v>
       </c>
       <c r="H1122">
         <v>0</v>
       </c>
       <c r="I1122">
-        <v>0.1</v>
+        <v>310625.5166666667</v>
       </c>
       <c r="J1122" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1122">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L1122" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA OKL_D</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U BPC_D</t>
         </is>
       </c>
       <c r="M1122" t="inlineStr">
         <is>
-          <t>backward</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="N1122" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1122" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P1122" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="1123">
       <c r="A1123" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E1189A4</t>
         </is>
       </c>
       <c r="B1123" t="inlineStr">
         <is>
-          <t>MRC_D</t>
+          <t>BPC_U</t>
         </is>
       </c>
       <c r="C1123">
@@ -68206,98 +68233,101 @@
         </is>
       </c>
       <c r="E1123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1123" s="2">
-        <v>45363.07224537037</v>
+        <v>45419.55506944444</v>
       </c>
       <c r="G1123" s="2">
-        <v>45363.07224537037</v>
+        <v>45419.55515046296</v>
       </c>
       <c r="H1123">
-        <v>0</v>
+        <v>0.1166666666666667</v>
       </c>
       <c r="I1123">
-        <v>17043.1</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="J1123" s="2">
-        <v>45100.64001157407</v>
+        <v>45181.30791666667</v>
       </c>
       <c r="K1123">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L1123" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="M1123" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="N1123" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
         </is>
       </c>
       <c r="O1123" t="b">
+        <v>1</v>
+      </c>
+      <c r="P1123" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1124">
       <c r="A1124" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1124" t="inlineStr">
         <is>
-          <t>CRW_D</t>
+          <t>PRA</t>
         </is>
       </c>
       <c r="C1124">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D1124" t="inlineStr">
         <is>
-          <t>Observation</t>
+          <t>Recapture</t>
         </is>
       </c>
       <c r="E1124">
         <v>2</v>
       </c>
       <c r="F1124" s="2">
-        <v>45369.91342592593</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="G1124" s="2">
-        <v>45369.91350694445</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="H1124">
-        <v>0.1166666666666667</v>
+        <v>0</v>
       </c>
       <c r="I1124">
-        <v>9851.299999999999</v>
+        <v>5797.566666666667</v>
       </c>
       <c r="J1124" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1124">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="L1124" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D MRC_U CRW_D</t>
+          <t>PRA</t>
         </is>
       </c>
       <c r="M1124" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>start</t>
         </is>
       </c>
       <c r="N1124" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1124" t="b">
@@ -68307,16 +68337,16 @@
     <row r="1125">
       <c r="A1125" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1125" t="inlineStr">
         <is>
-          <t>CRW_U</t>
+          <t>PRA</t>
         </is>
       </c>
       <c r="C1125">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1125" t="inlineStr">
         <is>
@@ -68324,39 +68354,39 @@
         </is>
       </c>
       <c r="E1125">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1125" s="2">
-        <v>45369.91527777778</v>
+        <v>45166.39038194445</v>
       </c>
       <c r="G1125" s="2">
-        <v>45369.91530092592</v>
+        <v>45166.39038194445</v>
       </c>
       <c r="H1125">
-        <v>0.03333333333333333</v>
+        <v>0</v>
       </c>
       <c r="I1125">
-        <v>2.55</v>
+        <v>5.3</v>
       </c>
       <c r="J1125" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1125">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L1125" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D MRC_U CRW_D CRW_U</t>
+          <t>PRA</t>
         </is>
       </c>
       <c r="M1125" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>no movement</t>
         </is>
       </c>
       <c r="N1125" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1125" t="b">
@@ -68366,16 +68396,16 @@
     <row r="1126">
       <c r="A1126" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1126" t="inlineStr">
         <is>
-          <t>CRU_U</t>
+          <t>RIA</t>
         </is>
       </c>
       <c r="C1126">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D1126" t="inlineStr">
         <is>
@@ -68383,29 +68413,29 @@
         </is>
       </c>
       <c r="E1126">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F1126" s="2">
-        <v>45384.89723379629</v>
+        <v>45168.85053240741</v>
       </c>
       <c r="G1126" s="2">
-        <v>45384.89723379629</v>
+        <v>45169.01416666667</v>
       </c>
       <c r="H1126">
-        <v>0</v>
+        <v>235.6333333333333</v>
       </c>
       <c r="I1126">
-        <v>20137.43333333333</v>
+        <v>3542.616666666667</v>
       </c>
       <c r="J1126" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1126">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="L1126" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D MRC_U CRW_D CRW_U CRU_D CRU_U</t>
+          <t>PRA RIA</t>
         </is>
       </c>
       <c r="M1126" t="inlineStr">
@@ -68415,26 +68445,26 @@
       </c>
       <c r="N1126" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1127">
       <c r="A1127" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1127" t="inlineStr">
         <is>
-          <t>CRU_D</t>
+          <t>RRF</t>
         </is>
       </c>
       <c r="C1127">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D1127" t="inlineStr">
         <is>
@@ -68442,39 +68472,39 @@
         </is>
       </c>
       <c r="E1127">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1127" s="2">
-        <v>45385.82677083333</v>
+        <v>45170.59445601852</v>
       </c>
       <c r="G1127" s="2">
-        <v>45385.82677083333</v>
+        <v>45170.59594907408</v>
       </c>
       <c r="H1127">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="I1127">
-        <v>1338.533333333333</v>
+        <v>2275.616666666667</v>
       </c>
       <c r="J1127" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1127">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="L1127" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D MRC_U CRW_D CRW_U CRU_D</t>
+          <t>PRA RIA RRF</t>
         </is>
       </c>
       <c r="M1127" t="inlineStr">
         <is>
-          <t>backward</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="N1127" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1127" t="b">
@@ -68484,16 +68514,16 @@
     <row r="1128">
       <c r="A1128" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1128" t="inlineStr">
         <is>
-          <t>CRU_U</t>
+          <t>WEA</t>
         </is>
       </c>
       <c r="C1128">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D1128" t="inlineStr">
         <is>
@@ -68501,29 +68531,29 @@
         </is>
       </c>
       <c r="E1128">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1128" s="2">
-        <v>45386.90662037037</v>
+        <v>45172.58729166667</v>
       </c>
       <c r="G1128" s="2">
-        <v>45387.17353009259</v>
+        <v>45172.66815972222</v>
       </c>
       <c r="H1128">
-        <v>384.35</v>
+        <v>116.45</v>
       </c>
       <c r="I1128">
-        <v>1554.983333333333</v>
+        <v>2867.533333333333</v>
       </c>
       <c r="J1128" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1128">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="L1128" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D MRC_U CRW_D CRW_U CRU_D CRU_U</t>
+          <t>PRA RIA RRF WEA</t>
         </is>
       </c>
       <c r="M1128" t="inlineStr">
@@ -68533,7 +68563,7 @@
       </c>
       <c r="N1128" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1128" t="b">
@@ -68543,16 +68573,16 @@
     <row r="1129">
       <c r="A1129" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1129" t="inlineStr">
         <is>
-          <t>CRU_D</t>
+          <t>OKL_D</t>
         </is>
       </c>
       <c r="C1129">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D1129" t="inlineStr">
         <is>
@@ -68560,58 +68590,58 @@
         </is>
       </c>
       <c r="E1129">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F1129" s="2">
-        <v>45387.17366898149</v>
+        <v>45186.08542824074</v>
       </c>
       <c r="G1129" s="2">
-        <v>45400.05799768519</v>
+        <v>45186.08542824074</v>
       </c>
       <c r="H1129">
-        <v>18553.43333333333</v>
+        <v>0</v>
       </c>
       <c r="I1129">
-        <v>0.2</v>
+        <v>19320.86666666666</v>
       </c>
       <c r="J1129" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1129">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="L1129" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA LMR_D LMR_U MRC_D MRC_U CRW_D CRW_U CRU_D</t>
+          <t>PRA RIA RRF WEA OKL_D</t>
         </is>
       </c>
       <c r="M1129" t="inlineStr">
         <is>
-          <t>backward</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="N1129" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1130">
       <c r="A1130" t="inlineStr">
         <is>
-          <t>3DD.003DE8629C</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1130" t="inlineStr">
         <is>
-          <t>RRF</t>
+          <t>WHS</t>
         </is>
       </c>
       <c r="C1130">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D1130" t="inlineStr">
         <is>
@@ -68619,39 +68649,39 @@
         </is>
       </c>
       <c r="E1130">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1130" s="2">
-        <v>45428.63291666667</v>
+        <v>45386.39444444445</v>
       </c>
       <c r="G1130" s="2">
-        <v>45428.63291666667</v>
+        <v>45387.17129629629</v>
       </c>
       <c r="H1130">
-        <v>0</v>
+        <v>1118.666666666667</v>
       </c>
       <c r="I1130">
-        <v>7594.533333333334</v>
+        <v>288444.9833333333</v>
       </c>
       <c r="J1130" s="2">
-        <v>45100.64001157407</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1130">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L1130" t="inlineStr">
         <is>
-          <t>PRA RIA RRF</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U WHS</t>
         </is>
       </c>
       <c r="M1130" t="inlineStr">
         <is>
-          <t>backward</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="N1130" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U OKL_D MRC_D CRW_D CRW_U CML CMU CRU_U CRU_D CRU_U CRU_D CML RRF</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1130" t="b">
@@ -68661,78 +68691,75 @@
     <row r="1131">
       <c r="A1131" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1131" t="inlineStr">
         <is>
-          <t>PRA</t>
+          <t>ANT_D</t>
         </is>
       </c>
       <c r="C1131">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1131" t="inlineStr">
         <is>
-          <t>Recapture</t>
+          <t>Observation</t>
         </is>
       </c>
       <c r="E1131">
         <v>1</v>
       </c>
       <c r="F1131" s="2">
-        <v>45181.30791666667</v>
+        <v>45388.14509259259</v>
       </c>
       <c r="G1131" s="2">
-        <v>45181.30791666667</v>
+        <v>45388.14509259259</v>
       </c>
       <c r="H1131">
         <v>0</v>
       </c>
       <c r="I1131">
-        <v>4.3</v>
+        <v>1402.266666666667</v>
       </c>
       <c r="J1131" s="2">
-        <v>45181.30791666667</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1131">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="L1131" t="inlineStr">
         <is>
-          <t>PRA</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
         </is>
       </c>
       <c r="M1131" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="N1131" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1131" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1131" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1132">
       <c r="A1132" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1132" t="inlineStr">
         <is>
-          <t>PRA</t>
+          <t>ANT_U</t>
         </is>
       </c>
       <c r="C1132">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1132" t="inlineStr">
         <is>
@@ -68740,61 +68767,58 @@
         </is>
       </c>
       <c r="E1132">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1132" s="2">
-        <v>45181.34018518518</v>
+        <v>45388.14642361111</v>
       </c>
       <c r="G1132" s="2">
-        <v>45181.34247685185</v>
+        <v>45388.14642361111</v>
       </c>
       <c r="H1132">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="I1132">
-        <v>46.46666666666667</v>
+        <v>1.916666666666667</v>
       </c>
       <c r="J1132" s="2">
-        <v>45181.30791666667</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1132">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L1132" t="inlineStr">
         <is>
-          <t>PRA</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D ANT_U</t>
         </is>
       </c>
       <c r="M1132" t="inlineStr">
         <is>
-          <t>no movement</t>
+          <t>forward</t>
         </is>
       </c>
       <c r="N1132" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1132" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1132" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1133">
       <c r="A1133" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1133" t="inlineStr">
         <is>
-          <t>RIA</t>
+          <t>ANT_D</t>
         </is>
       </c>
       <c r="C1133">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D1133" t="inlineStr">
         <is>
@@ -68802,61 +68826,58 @@
         </is>
       </c>
       <c r="E1133">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F1133" s="2">
-        <v>45186.11847222222</v>
+        <v>45402.24827546296</v>
       </c>
       <c r="G1133" s="2">
-        <v>45186.16163194444</v>
+        <v>45402.24827546296</v>
       </c>
       <c r="H1133">
-        <v>62.15</v>
+        <v>0</v>
       </c>
       <c r="I1133">
-        <v>6877.433333333333</v>
+        <v>20306.66666666667</v>
       </c>
       <c r="J1133" s="2">
-        <v>45181.30791666667</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1133">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L1133" t="inlineStr">
         <is>
-          <t>PRA RIA</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
         </is>
       </c>
       <c r="M1133" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>backward</t>
         </is>
       </c>
       <c r="N1133" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1133" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1133" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1134">
       <c r="A1134" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1134" t="inlineStr">
         <is>
-          <t>RRF</t>
+          <t>WHS</t>
         </is>
       </c>
       <c r="C1134">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D1134" t="inlineStr">
         <is>
@@ -68864,61 +68885,58 @@
         </is>
       </c>
       <c r="E1134">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1134" s="2">
-        <v>45187.44148148148</v>
+        <v>45405.65003472222</v>
       </c>
       <c r="G1134" s="2">
-        <v>45187.45084490741</v>
+        <v>45409.69375</v>
       </c>
       <c r="H1134">
-        <v>13.48333333333333</v>
+        <v>5822.95</v>
       </c>
       <c r="I1134">
-        <v>1842.983333333333</v>
+        <v>4898.533333333334</v>
       </c>
       <c r="J1134" s="2">
-        <v>45181.30791666667</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1134">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L1134" t="inlineStr">
         <is>
-          <t>PRA RIA RRF</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U WHS</t>
         </is>
       </c>
       <c r="M1134" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="N1134" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1134" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1134" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1135">
       <c r="A1135" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1135" t="inlineStr">
         <is>
-          <t>WEA</t>
+          <t>ANT_D</t>
         </is>
       </c>
       <c r="C1135">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D1135" t="inlineStr">
         <is>
@@ -68926,61 +68944,58 @@
         </is>
       </c>
       <c r="E1135">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F1135" s="2">
-        <v>45189.72104166666</v>
+        <v>45411.71814814815</v>
       </c>
       <c r="G1135" s="2">
-        <v>45189.77603009259</v>
+        <v>45411.71814814815</v>
       </c>
       <c r="H1135">
-        <v>79.18333333333334</v>
+        <v>0</v>
       </c>
       <c r="I1135">
-        <v>3269.083333333333</v>
+        <v>2915.133333333333</v>
       </c>
       <c r="J1135" s="2">
-        <v>45181.30791666667</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1135">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L1135" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
         </is>
       </c>
       <c r="M1135" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="N1135" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1135" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1135" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1136">
       <c r="A1136" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1136" t="inlineStr">
         <is>
-          <t>OKL_D</t>
+          <t>ANT_U</t>
         </is>
       </c>
       <c r="C1136">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D1136" t="inlineStr">
         <is>
@@ -68991,26 +69006,26 @@
         <v>1</v>
       </c>
       <c r="F1136" s="2">
-        <v>45203.8422337963</v>
+        <v>45413.55326388888</v>
       </c>
       <c r="G1136" s="2">
-        <v>45203.8422337963</v>
+        <v>45413.55326388888</v>
       </c>
       <c r="H1136">
         <v>0</v>
       </c>
       <c r="I1136">
-        <v>20255.33333333333</v>
+        <v>2642.566666666667</v>
       </c>
       <c r="J1136" s="2">
-        <v>45181.30791666667</v>
+        <v>45166.38670138889</v>
       </c>
       <c r="K1136">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L1136" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA OKL_D</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D ANT_U</t>
         </is>
       </c>
       <c r="M1136" t="inlineStr">
@@ -69020,1025 +69035,69 @@
       </c>
       <c r="N1136" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1136" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1136" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="1137">
       <c r="A1137" t="inlineStr">
         <is>
-          <t>3DD.003E1189A4</t>
+          <t>3DD.003E16C1E6</t>
         </is>
       </c>
       <c r="B1137" t="inlineStr">
         <is>
-          <t>OKL_U</t>
+          <t>ANT_D</t>
         </is>
       </c>
       <c r="C1137">
+        <v>14</v>
+      </c>
+      <c r="D1137" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="E1137">
+        <v>1</v>
+      </c>
+      <c r="F1137" s="2">
+        <v>45413.55362268518</v>
+      </c>
+      <c r="G1137" s="2">
+        <v>45413.55362268518</v>
+      </c>
+      <c r="H1137">
+        <v>0</v>
+      </c>
+      <c r="I1137">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="J1137" s="2">
+        <v>45166.38670138889</v>
+      </c>
+      <c r="K1137">
         <v>7</v>
       </c>
-      <c r="D1137" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1137">
-        <v>1</v>
-      </c>
-      <c r="F1137" s="2">
-        <v>45203.84256944444</v>
-      </c>
-      <c r="G1137" s="2">
-        <v>45203.84256944444</v>
-      </c>
-      <c r="H1137">
-        <v>0</v>
-      </c>
-      <c r="I1137">
-        <v>0.4833333333333333</v>
-      </c>
-      <c r="J1137" s="2">
-        <v>45181.30791666667</v>
-      </c>
-      <c r="K1137">
-        <v>6</v>
-      </c>
       <c r="L1137" t="inlineStr">
         <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U</t>
+          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
         </is>
       </c>
       <c r="M1137" t="inlineStr">
         <is>
-          <t>forward</t>
+          <t>backward</t>
         </is>
       </c>
       <c r="N1137" t="inlineStr">
         <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
+          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
         </is>
       </c>
       <c r="O1137" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1137" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1138">
-      <c r="A1138" t="inlineStr">
-        <is>
-          <t>3DD.003E1189A4</t>
-        </is>
-      </c>
-      <c r="B1138" t="inlineStr">
-        <is>
-          <t>BPC_D</t>
-        </is>
-      </c>
-      <c r="C1138">
-        <v>8</v>
-      </c>
-      <c r="D1138" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1138">
-        <v>1</v>
-      </c>
-      <c r="F1138" s="2">
-        <v>45419.55473379629</v>
-      </c>
-      <c r="G1138" s="2">
-        <v>45419.55473379629</v>
-      </c>
-      <c r="H1138">
-        <v>0</v>
-      </c>
-      <c r="I1138">
-        <v>310625.5166666667</v>
-      </c>
-      <c r="J1138" s="2">
-        <v>45181.30791666667</v>
-      </c>
-      <c r="K1138">
-        <v>7</v>
-      </c>
-      <c r="L1138" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U BPC_D</t>
-        </is>
-      </c>
-      <c r="M1138" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1138" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
-        </is>
-      </c>
-      <c r="O1138" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1138" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1139">
-      <c r="A1139" t="inlineStr">
-        <is>
-          <t>3DD.003E1189A4</t>
-        </is>
-      </c>
-      <c r="B1139" t="inlineStr">
-        <is>
-          <t>BPC_U</t>
-        </is>
-      </c>
-      <c r="C1139">
-        <v>9</v>
-      </c>
-      <c r="D1139" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1139">
-        <v>2</v>
-      </c>
-      <c r="F1139" s="2">
-        <v>45419.55506944444</v>
-      </c>
-      <c r="G1139" s="2">
-        <v>45419.55515046296</v>
-      </c>
-      <c r="H1139">
-        <v>0.1166666666666667</v>
-      </c>
-      <c r="I1139">
-        <v>0.4833333333333333</v>
-      </c>
-      <c r="J1139" s="2">
-        <v>45181.30791666667</v>
-      </c>
-      <c r="K1139">
-        <v>8</v>
-      </c>
-      <c r="L1139" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
-        </is>
-      </c>
-      <c r="M1139" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1139" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D OKL_U BPC_D BPC_U</t>
-        </is>
-      </c>
-      <c r="O1139" t="b">
-        <v>1</v>
-      </c>
-      <c r="P1139" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1140">
-      <c r="A1140" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1140" t="inlineStr">
-        <is>
-          <t>PRA</t>
-        </is>
-      </c>
-      <c r="C1140">
-        <v>1</v>
-      </c>
-      <c r="D1140" t="inlineStr">
-        <is>
-          <t>Recapture</t>
-        </is>
-      </c>
-      <c r="E1140">
-        <v>2</v>
-      </c>
-      <c r="F1140" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="G1140" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="H1140">
-        <v>0</v>
-      </c>
-      <c r="I1140">
-        <v>5797.566666666667</v>
-      </c>
-      <c r="J1140" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1140">
-        <v>1</v>
-      </c>
-      <c r="L1140" t="inlineStr">
-        <is>
-          <t>PRA</t>
-        </is>
-      </c>
-      <c r="M1140" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="N1140" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1140" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1141">
-      <c r="A1141" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1141" t="inlineStr">
-        <is>
-          <t>PRA</t>
-        </is>
-      </c>
-      <c r="C1141">
-        <v>2</v>
-      </c>
-      <c r="D1141" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1141">
-        <v>3</v>
-      </c>
-      <c r="F1141" s="2">
-        <v>45166.39038194445</v>
-      </c>
-      <c r="G1141" s="2">
-        <v>45166.39038194445</v>
-      </c>
-      <c r="H1141">
-        <v>0</v>
-      </c>
-      <c r="I1141">
-        <v>5.3</v>
-      </c>
-      <c r="J1141" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1141">
-        <v>1</v>
-      </c>
-      <c r="L1141" t="inlineStr">
-        <is>
-          <t>PRA</t>
-        </is>
-      </c>
-      <c r="M1141" t="inlineStr">
-        <is>
-          <t>no movement</t>
-        </is>
-      </c>
-      <c r="N1141" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1141" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1142">
-      <c r="A1142" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1142" t="inlineStr">
-        <is>
-          <t>RIA</t>
-        </is>
-      </c>
-      <c r="C1142">
-        <v>3</v>
-      </c>
-      <c r="D1142" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1142">
-        <v>18</v>
-      </c>
-      <c r="F1142" s="2">
-        <v>45168.85053240741</v>
-      </c>
-      <c r="G1142" s="2">
-        <v>45169.01416666667</v>
-      </c>
-      <c r="H1142">
-        <v>235.6333333333333</v>
-      </c>
-      <c r="I1142">
-        <v>3542.616666666667</v>
-      </c>
-      <c r="J1142" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1142">
-        <v>2</v>
-      </c>
-      <c r="L1142" t="inlineStr">
-        <is>
-          <t>PRA RIA</t>
-        </is>
-      </c>
-      <c r="M1142" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1142" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1142" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1143">
-      <c r="A1143" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1143" t="inlineStr">
-        <is>
-          <t>RRF</t>
-        </is>
-      </c>
-      <c r="C1143">
-        <v>4</v>
-      </c>
-      <c r="D1143" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1143">
-        <v>2</v>
-      </c>
-      <c r="F1143" s="2">
-        <v>45170.59445601852</v>
-      </c>
-      <c r="G1143" s="2">
-        <v>45170.59594907408</v>
-      </c>
-      <c r="H1143">
-        <v>2.15</v>
-      </c>
-      <c r="I1143">
-        <v>2275.616666666667</v>
-      </c>
-      <c r="J1143" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1143">
-        <v>3</v>
-      </c>
-      <c r="L1143" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF</t>
-        </is>
-      </c>
-      <c r="M1143" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1143" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1143" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1144">
-      <c r="A1144" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1144" t="inlineStr">
-        <is>
-          <t>WEA</t>
-        </is>
-      </c>
-      <c r="C1144">
-        <v>5</v>
-      </c>
-      <c r="D1144" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1144">
-        <v>3</v>
-      </c>
-      <c r="F1144" s="2">
-        <v>45172.58729166667</v>
-      </c>
-      <c r="G1144" s="2">
-        <v>45172.66815972222</v>
-      </c>
-      <c r="H1144">
-        <v>116.45</v>
-      </c>
-      <c r="I1144">
-        <v>2867.533333333333</v>
-      </c>
-      <c r="J1144" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1144">
-        <v>4</v>
-      </c>
-      <c r="L1144" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA</t>
-        </is>
-      </c>
-      <c r="M1144" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1144" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1144" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1145">
-      <c r="A1145" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1145" t="inlineStr">
-        <is>
-          <t>OKL_D</t>
-        </is>
-      </c>
-      <c r="C1145">
-        <v>6</v>
-      </c>
-      <c r="D1145" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1145">
-        <v>1</v>
-      </c>
-      <c r="F1145" s="2">
-        <v>45186.08542824074</v>
-      </c>
-      <c r="G1145" s="2">
-        <v>45186.08542824074</v>
-      </c>
-      <c r="H1145">
-        <v>0</v>
-      </c>
-      <c r="I1145">
-        <v>19320.86666666666</v>
-      </c>
-      <c r="J1145" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1145">
-        <v>5</v>
-      </c>
-      <c r="L1145" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D</t>
-        </is>
-      </c>
-      <c r="M1145" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1145" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1145" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1146">
-      <c r="A1146" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1146" t="inlineStr">
-        <is>
-          <t>WHS</t>
-        </is>
-      </c>
-      <c r="C1146">
-        <v>7</v>
-      </c>
-      <c r="D1146" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1146">
-        <v>2</v>
-      </c>
-      <c r="F1146" s="2">
-        <v>45386.39444444445</v>
-      </c>
-      <c r="G1146" s="2">
-        <v>45387.17129629629</v>
-      </c>
-      <c r="H1146">
-        <v>1118.666666666667</v>
-      </c>
-      <c r="I1146">
-        <v>288444.9833333333</v>
-      </c>
-      <c r="J1146" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1146">
-        <v>7</v>
-      </c>
-      <c r="L1146" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U WHS</t>
-        </is>
-      </c>
-      <c r="M1146" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1146" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1146" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1147">
-      <c r="A1147" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1147" t="inlineStr">
-        <is>
-          <t>ANT_D</t>
-        </is>
-      </c>
-      <c r="C1147">
-        <v>8</v>
-      </c>
-      <c r="D1147" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1147">
-        <v>1</v>
-      </c>
-      <c r="F1147" s="2">
-        <v>45388.14509259259</v>
-      </c>
-      <c r="G1147" s="2">
-        <v>45388.14509259259</v>
-      </c>
-      <c r="H1147">
-        <v>0</v>
-      </c>
-      <c r="I1147">
-        <v>1402.266666666667</v>
-      </c>
-      <c r="J1147" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1147">
-        <v>7</v>
-      </c>
-      <c r="L1147" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
-        </is>
-      </c>
-      <c r="M1147" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="N1147" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1147" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1148">
-      <c r="A1148" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1148" t="inlineStr">
-        <is>
-          <t>ANT_U</t>
-        </is>
-      </c>
-      <c r="C1148">
-        <v>9</v>
-      </c>
-      <c r="D1148" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1148">
-        <v>1</v>
-      </c>
-      <c r="F1148" s="2">
-        <v>45388.14642361111</v>
-      </c>
-      <c r="G1148" s="2">
-        <v>45388.14642361111</v>
-      </c>
-      <c r="H1148">
-        <v>0</v>
-      </c>
-      <c r="I1148">
-        <v>1.916666666666667</v>
-      </c>
-      <c r="J1148" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1148">
-        <v>8</v>
-      </c>
-      <c r="L1148" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D ANT_U</t>
-        </is>
-      </c>
-      <c r="M1148" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1148" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1148" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1149">
-      <c r="A1149" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1149" t="inlineStr">
-        <is>
-          <t>ANT_D</t>
-        </is>
-      </c>
-      <c r="C1149">
-        <v>10</v>
-      </c>
-      <c r="D1149" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1149">
-        <v>1</v>
-      </c>
-      <c r="F1149" s="2">
-        <v>45402.24827546296</v>
-      </c>
-      <c r="G1149" s="2">
-        <v>45402.24827546296</v>
-      </c>
-      <c r="H1149">
-        <v>0</v>
-      </c>
-      <c r="I1149">
-        <v>20306.66666666667</v>
-      </c>
-      <c r="J1149" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1149">
-        <v>7</v>
-      </c>
-      <c r="L1149" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
-        </is>
-      </c>
-      <c r="M1149" t="inlineStr">
-        <is>
-          <t>backward</t>
-        </is>
-      </c>
-      <c r="N1149" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1149" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1150">
-      <c r="A1150" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1150" t="inlineStr">
-        <is>
-          <t>WHS</t>
-        </is>
-      </c>
-      <c r="C1150">
-        <v>11</v>
-      </c>
-      <c r="D1150" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1150">
-        <v>11</v>
-      </c>
-      <c r="F1150" s="2">
-        <v>45405.65003472222</v>
-      </c>
-      <c r="G1150" s="2">
-        <v>45409.69375</v>
-      </c>
-      <c r="H1150">
-        <v>5822.95</v>
-      </c>
-      <c r="I1150">
-        <v>4898.533333333334</v>
-      </c>
-      <c r="J1150" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1150">
-        <v>7</v>
-      </c>
-      <c r="L1150" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U WHS</t>
-        </is>
-      </c>
-      <c r="M1150" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="N1150" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1150" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1151">
-      <c r="A1151" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1151" t="inlineStr">
-        <is>
-          <t>ANT_D</t>
-        </is>
-      </c>
-      <c r="C1151">
-        <v>12</v>
-      </c>
-      <c r="D1151" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1151">
-        <v>1</v>
-      </c>
-      <c r="F1151" s="2">
-        <v>45411.71814814815</v>
-      </c>
-      <c r="G1151" s="2">
-        <v>45411.71814814815</v>
-      </c>
-      <c r="H1151">
-        <v>0</v>
-      </c>
-      <c r="I1151">
-        <v>2915.133333333333</v>
-      </c>
-      <c r="J1151" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1151">
-        <v>7</v>
-      </c>
-      <c r="L1151" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
-        </is>
-      </c>
-      <c r="M1151" t="inlineStr">
-        <is>
-          <t>unknown</t>
-        </is>
-      </c>
-      <c r="N1151" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1151" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1152">
-      <c r="A1152" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1152" t="inlineStr">
-        <is>
-          <t>ANT_U</t>
-        </is>
-      </c>
-      <c r="C1152">
-        <v>13</v>
-      </c>
-      <c r="D1152" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1152">
-        <v>1</v>
-      </c>
-      <c r="F1152" s="2">
-        <v>45413.55326388888</v>
-      </c>
-      <c r="G1152" s="2">
-        <v>45413.55326388888</v>
-      </c>
-      <c r="H1152">
-        <v>0</v>
-      </c>
-      <c r="I1152">
-        <v>2642.566666666667</v>
-      </c>
-      <c r="J1152" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1152">
-        <v>8</v>
-      </c>
-      <c r="L1152" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D ANT_U</t>
-        </is>
-      </c>
-      <c r="M1152" t="inlineStr">
-        <is>
-          <t>forward</t>
-        </is>
-      </c>
-      <c r="N1152" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1152" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1153">
-      <c r="A1153" t="inlineStr">
-        <is>
-          <t>3DD.003E16C1E6</t>
-        </is>
-      </c>
-      <c r="B1153" t="inlineStr">
-        <is>
-          <t>ANT_D</t>
-        </is>
-      </c>
-      <c r="C1153">
-        <v>14</v>
-      </c>
-      <c r="D1153" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="E1153">
-        <v>1</v>
-      </c>
-      <c r="F1153" s="2">
-        <v>45413.55362268518</v>
-      </c>
-      <c r="G1153" s="2">
-        <v>45413.55362268518</v>
-      </c>
-      <c r="H1153">
-        <v>0</v>
-      </c>
-      <c r="I1153">
-        <v>0.5166666666666667</v>
-      </c>
-      <c r="J1153" s="2">
-        <v>45166.38670138889</v>
-      </c>
-      <c r="K1153">
-        <v>7</v>
-      </c>
-      <c r="L1153" t="inlineStr">
-        <is>
-          <t>PRA RIA RRF WEA OKL_D OKL_U ANT_D</t>
-        </is>
-      </c>
-      <c r="M1153" t="inlineStr">
-        <is>
-          <t>backward</t>
-        </is>
-      </c>
-      <c r="N1153" t="inlineStr">
-        <is>
-          <t>PRA PRA RIA RRF WEA OKL_D WHS ANT_D ANT_U ANT_D WHS ANT_D ANT_U ANT_D</t>
-        </is>
-      </c>
-      <c r="O1153" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>